<commit_message>
feat: updated question presentation format
</commit_message>
<xml_diff>
--- a/stimuli_toy/multipleye_comprehension_questions_toy.xlsx
+++ b/stimuli_toy/multipleye_comprehension_questions_toy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/debor/repos/wg1-image-creation/stimuli_toy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E8DD672-F6A4-6646-9431-A82C54601112}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EF14704-75B6-6144-9C74-4364810D53F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="23500" xr2:uid="{BF0A98E9-F8D9-4949-AD77-1583D2976307}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="29920" windowHeight="18660" xr2:uid="{BF0A98E9-F8D9-4949-AD77-1583D2976307}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="45">
   <si>
     <t>stimulus_id</t>
   </si>
@@ -117,9 +117,6 @@
   </si>
   <si>
     <t>distractor_1_span_text</t>
-  </si>
-  <si>
-    <t>From what book and by whom is this passage?</t>
   </si>
   <si>
     <t>George Eliot - Middlemarch</t>
@@ -241,9 +238,6 @@
 Eye movements in reading are known to reflect cognitive processes involved in reading comprehension at all linguistic levels, from the sub-lexical to the discourse level. This means that reading comprehension and other properties of the text and/or the reader should be possible to infer from eye movements. Consequently, we develop the first neural sequence architecture for this type of tasks which models scan paths in reading and incorporates lexical, semantic and other linguistic features of the stimulus text. Our proposed model outperforms state-of-the-art models in various tasks. </t>
   </si>
   <si>
-    <t>What can be infred from eye-movements?</t>
-  </si>
-  <si>
     <t>Reading comprehension</t>
   </si>
   <si>
@@ -285,6 +279,21 @@
       </rPr>
       <t xml:space="preserve">$ and other properties of the text and/or the reader should be possible to infer from eye movements. Consequently, we develop the first neural sequence architecture for this type of tasks which models scan paths in reading and incorporates lexical, semantic and other linguistic features of the stimulus text. Our proposed model outperforms state-of-the-art models in various tasks. </t>
     </r>
+  </si>
+  <si>
+    <t>What can be infered from eye-movements?</t>
+  </si>
+  <si>
+    <t>whatever</t>
+  </si>
+  <si>
+    <t>watever</t>
+  </si>
+  <si>
+    <t>and this is another very long answer option to test what happens</t>
+  </si>
+  <si>
+    <t>This is a very long question that is completely useless, but we need it to test how a two-line question looks like!</t>
   </si>
 </sst>
 </file>
@@ -389,7 +398,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -406,9 +415,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -747,8 +753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{899C6EA3-68FC-004D-97A8-DCDE2573704E}">
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -814,37 +820,37 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" t="s">
         <v>28</v>
       </c>
-      <c r="F2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I2" t="s">
-        <v>26</v>
-      </c>
-      <c r="J2" t="s">
-        <v>25</v>
-      </c>
-      <c r="K2" t="s">
-        <v>27</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>29</v>
-      </c>
-      <c r="M2" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="272" x14ac:dyDescent="0.2">
@@ -855,22 +861,31 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s">
         <v>3</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I3" t="s">
         <v>41</v>
       </c>
-      <c r="F3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" t="s">
-        <v>40</v>
+      <c r="J3" t="s">
+        <v>42</v>
+      </c>
+      <c r="K3" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="272" x14ac:dyDescent="0.2">
@@ -881,34 +896,37 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D4" t="s">
         <v>3</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H4" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J4" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="I4" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="J4" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="L4" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="M4" s="10" t="s">
-        <v>20</v>
+      <c r="K4" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="221" x14ac:dyDescent="0.2">
@@ -919,37 +937,37 @@
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D5" t="s">
         <v>2</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F5" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" s="4" t="s">
+      <c r="I5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="J5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="K5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="K5" s="4" t="s">
+      <c r="L5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="L5" s="4" t="s">
-        <v>20</v>
-      </c>
       <c r="M5" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">

</xml_diff>